<commit_message>
Added sidebar and data visualization.
</commit_message>
<xml_diff>
--- a/PythonProjectDataset.xlsx
+++ b/PythonProjectDataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukep\Documents\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4225111-0E04-49C2-9508-08C8D1296083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933440F4-916A-4CBA-89A3-07BF45605635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A675823-8B8F-4073-814D-D801FD81B268}"/>
   </bookViews>
@@ -344,8 +344,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,7 +664,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,7 +673,7 @@
     <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" customWidth="1"/>
   </cols>
@@ -690,7 +691,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -713,7 +714,7 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>2017</v>
       </c>
       <c r="F2" t="s">
@@ -736,7 +737,7 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>2018</v>
       </c>
       <c r="F3" t="s">
@@ -759,7 +760,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>2017</v>
       </c>
       <c r="F4" t="s">
@@ -782,7 +783,7 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>2015</v>
       </c>
       <c r="F5" t="s">
@@ -805,7 +806,7 @@
       <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>2019</v>
       </c>
       <c r="F6" t="s">
@@ -828,7 +829,7 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>2018</v>
       </c>
       <c r="F7" t="s">
@@ -851,7 +852,7 @@
       <c r="D8" t="s">
         <v>39</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>2020</v>
       </c>
       <c r="F8" t="s">
@@ -874,7 +875,7 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>2015</v>
       </c>
       <c r="F9" t="s">
@@ -897,7 +898,7 @@
       <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>2019</v>
       </c>
       <c r="F10" t="s">
@@ -920,7 +921,7 @@
       <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>2018</v>
       </c>
       <c r="F11" t="s">
@@ -943,7 +944,7 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>2015</v>
       </c>
       <c r="F12" t="s">
@@ -966,7 +967,7 @@
       <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>2020</v>
       </c>
       <c r="F13" t="s">
@@ -989,7 +990,7 @@
       <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>2020</v>
       </c>
       <c r="F14" t="s">
@@ -1012,7 +1013,7 @@
       <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>2020</v>
       </c>
       <c r="F15" t="s">
@@ -1035,7 +1036,7 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>2017</v>
       </c>
       <c r="F16" t="s">
@@ -1058,7 +1059,7 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>2016</v>
       </c>
       <c r="F17" t="s">
@@ -1081,7 +1082,7 @@
       <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>2016</v>
       </c>
       <c r="F18" t="s">
@@ -1104,7 +1105,7 @@
       <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>2019</v>
       </c>
       <c r="F19" t="s">
@@ -1127,7 +1128,7 @@
       <c r="D20" t="s">
         <v>74</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>2019</v>
       </c>
       <c r="F20" t="s">
@@ -1150,7 +1151,7 @@
       <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>2016</v>
       </c>
       <c r="F21" t="s">
@@ -1173,7 +1174,7 @@
       <c r="D22" t="s">
         <v>81</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>2018</v>
       </c>
       <c r="F22" t="s">
@@ -1196,7 +1197,7 @@
       <c r="D23" t="s">
         <v>81</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>2018</v>
       </c>
       <c r="F23" t="s">
@@ -1219,7 +1220,7 @@
       <c r="D24" t="s">
         <v>85</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>2015</v>
       </c>
       <c r="F24" t="s">
@@ -1242,7 +1243,7 @@
       <c r="D25" t="s">
         <v>90</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>2020</v>
       </c>
       <c r="F25" t="s">

</xml_diff>